<commit_message>
Creating beautiful tables in R with {gt}
</commit_message>
<xml_diff>
--- a/tables/books_eng.xlsx
+++ b/tables/books_eng.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@GitProjects/@2024/rsources-book/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FA794A-C9C9-0A40-9013-7046BFCAF856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705F274D-1F74-F34A-9D44-B46C265D7F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="500" windowWidth="25540" windowHeight="14160" xr2:uid="{D3150169-A0ED-F142-9C13-F6AF1A7F6BF6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="187">
   <si>
     <t>link</t>
   </si>
@@ -587,6 +587,15 @@
   </si>
   <si>
     <t>Allen B. Downey</t>
+  </si>
+  <si>
+    <t>Creating beautiful tables in R with {gt}</t>
+  </si>
+  <si>
+    <t>https://gt.albert-rapp.de/</t>
+  </si>
+  <si>
+    <t>Albert Rapp</t>
   </si>
 </sst>
 </file>
@@ -942,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030A72B4-BCD4-C841-B970-1A2BD7901864}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C58" sqref="A58:C58"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1647,6 +1656,17 @@
         <v>174</v>
       </c>
     </row>
+    <row r="64" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>